<commit_message>
Lab2: Add GeoHash encodeHash/decodeHash methods.
</commit_message>
<xml_diff>
--- a/Lab2 (ISP test case design).xlsx
+++ b/Lab2 (ISP test case design).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="38400" windowHeight="19620"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="160">
   <si>
     <t>Method</t>
   </si>
@@ -366,64 +366,24 @@
     <t>Return the adjacent hash to the bottom (south).</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C11: id is null.</t>
-  </si>
-  <si>
-    <t>C11: {true, false}</t>
-  </si>
-  <si>
-    <t>T33: covers {true},
-T34: covers {false}</t>
-  </si>
-  <si>
     <t>lat()</t>
   </si>
   <si>
     <t>double</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C12: latitude's value.</t>
-  </si>
-  <si>
-    <t>C12: {latitude&lt;0, latitude=0, latitude&gt;0}</t>
-  </si>
-  <si>
     <t>{latitude&lt;0, latitude=0, latitude&gt;0}</t>
   </si>
   <si>
-    <t>T35: covers {latitude&lt;0},
-T36: covers {latitude=0},
-T37: covers {latitude&gt;0}</t>
-  </si>
-  <si>
-    <t>T35: {latitude=-23.25},
-T36: {latitude=0},
-T37: {latitude=23.25}</t>
-  </si>
-  <si>
     <t>lon()</t>
   </si>
   <si>
     <t>C13</t>
   </si>
   <si>
-    <t>C13: longitude's value.</t>
-  </si>
-  <si>
     <t>{longitude&lt;0, longitude=0, longitude&gt;0}</t>
   </si>
   <si>
-    <t>T38: covers {longitude&lt;0},
-T39: covers {longitude=0},
-T40: covers {longitude&gt;0}</t>
-  </si>
-  <si>
     <t>Return the corresponding id of Info.</t>
   </si>
   <si>
@@ -442,28 +402,9 @@
     <t>C14</t>
   </si>
   <si>
-    <t>C14: time's value.</t>
-  </si>
-  <si>
-    <t>C14: {time&lt;0, time=0, time&gt;0}</t>
-  </si>
-  <si>
-    <t>C13: {longitude&lt;0, longitude=0, longitude&gt;0}</t>
-  </si>
-  <si>
     <t>{time&lt;0, time=0, time&gt;0}</t>
   </si>
   <si>
-    <t>T41: {time=-123},
-T42: {time=0},
-T43: {time=123}</t>
-  </si>
-  <si>
-    <t>T41: covers {time&lt;0},
-T42: covers {time=0},
-T43: covers {time&gt;0}</t>
-  </si>
-  <si>
     <t>Info</t>
   </si>
   <si>
@@ -477,13 +418,6 @@
   </si>
   <si>
     <t>C15</t>
-  </si>
-  <si>
-    <t>C15: {true, false}</t>
-  </si>
-  <si>
-    <t>T33: {T=Integer, id=null},
-T34: {T=Integer, id=30}</t>
   </si>
   <si>
     <t>T44: covers {true},
@@ -499,20 +433,6 @@
     <t>C16</t>
   </si>
   <si>
-    <t>C16: Input Info's id is null.</t>
-  </si>
-  <si>
-    <t>C16: {true, false}</t>
-  </si>
-  <si>
-    <t>T46: {Info&lt;String, Integer&gt; (23.25, 120.55, 123, "2", Optional.of(null))},
-T47: {Info&lt;String, Integer&gt; (23.25, 120.55, 123, "2", Optional.of(30))}</t>
-  </si>
-  <si>
-    <t>T46: covers {true},
-T47: covers {false}</t>
-  </si>
-  <si>
     <t>Test Requirements
 (All Combination Coverage)</t>
   </si>
@@ -553,16 +473,180 @@
 T32: {hash=29jw}</t>
   </si>
   <si>
-    <t>T38: {longitude=-120.55},
-T39: {longitude=0},
-T40: {longitude=120.55}</t>
-  </si>
-  <si>
-    <t>C15: Input value is empty string.</t>
-  </si>
-  <si>
-    <t>T44: {R=String, value=empty string},
-T45: {R=String, value=2}</t>
+    <t>double latitude, double longitude, int length</t>
+  </si>
+  <si>
+    <t>encodeHash()</t>
+  </si>
+  <si>
+    <t>Return the geohash of given length for the given point.</t>
+  </si>
+  <si>
+    <t>C11, C12</t>
+  </si>
+  <si>
+    <t>C11: latitude's value.
+C12: longitude's value</t>
+  </si>
+  <si>
+    <t>C11: {-90=&lt;latitude&lt;0, latitude=0, 0&lt;latitude&lt;=90}
+C12: {-180=&lt;latitude&lt;0, latitude=0, 0&lt;latitude&lt;=180}</t>
+  </si>
+  <si>
+    <t>{
+-90=&lt;latitude&lt;0, -180=&lt;latitude&lt;0
+-90=&lt;latitude&lt;0, latitude=0
+-90=&lt;latitude&lt;0,  0&lt;latitude&lt;=180
+latitude=0, -180=&lt;latitude&lt;0
+latitude=0, latitude=0
+latitude=0, 0&lt;latitude&lt;=180
+0&lt;latitude&lt;=90, -180=&lt;latitude&lt;0
+0&lt;latitude&lt;=90, latitude=0
+0&lt;latitude&lt;=90, 0&lt;latitude&lt;=180
+}</t>
+  </si>
+  <si>
+    <t>T33: {latitude=-90, longtitude=-180, length=4},
+T34: {latitude=-90, longtitude=0, length=4},
+T35: {latitude=-90, longtitude=180, length=4},
+T36: {latitude=0, longtitude=-180, length=4},
+T37: {latitude=0, longtitude=0, length=4},
+T38: {latitude=0, longtitude=180, length=4},
+T39: {latitude=90, longtitude=-180, length=4},
+T40: {latitude=90, longtitude=0, length=4},
+T41: {latitude=90, longtitude=180, length=4}</t>
+  </si>
+  <si>
+    <t>T33: covers {-90=&lt;latitude&lt;0, -180=&lt;latitude&lt;0},
+T34: covers {-90=&lt;latitude&lt;0, latitude=0},
+T35: covers {-90=&lt;latitude&lt;0,  0&lt;latitude&lt;=180},
+T36: covers {latitude=0, -180=&lt;latitude&lt;0},
+T37: covers {latitude=0, latitude=0},
+T38: covers {latitude=0, 0&lt;latitude&lt;=180},
+T39: covers {0&lt;latitude&lt;=90, -180=&lt;latitude&lt;0},
+T40: covers {0&lt;latitude&lt;=90, latitude=0},
+T41: covers {0&lt;latitude&lt;=90, 0&lt;latitude&lt;=180}</t>
+  </si>
+  <si>
+    <t>decodeHash()</t>
+  </si>
+  <si>
+    <t>String geohash</t>
+  </si>
+  <si>
+    <t>LatLong</t>
+  </si>
+  <si>
+    <t>Returns a latitude,longitude pair as the centre of the given geohash.</t>
+  </si>
+  <si>
+    <t>C13: Input hash is null.</t>
+  </si>
+  <si>
+    <t>C13: {true, false}</t>
+  </si>
+  <si>
+    <t>T42: covers {true},
+T43: covers {false}</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C14: id is null.</t>
+  </si>
+  <si>
+    <t>C15: latitude's value.</t>
+  </si>
+  <si>
+    <t>C16: longitude's value.</t>
+  </si>
+  <si>
+    <t>C17: time's value.</t>
+  </si>
+  <si>
+    <t>C18: Input value is empty string.</t>
+  </si>
+  <si>
+    <t>C19: Input Info's id is null.</t>
+  </si>
+  <si>
+    <t>C14: {true, false}</t>
+  </si>
+  <si>
+    <t>C15: {latitude&lt;0, latitude=0, latitude&gt;0}</t>
+  </si>
+  <si>
+    <t>C16: {longitude&lt;0, longitude=0, longitude&gt;0}</t>
+  </si>
+  <si>
+    <t>C17: {time&lt;0, time=0, time&gt;0}</t>
+  </si>
+  <si>
+    <t>C18: {true, false}</t>
+  </si>
+  <si>
+    <t>C19: {true, false}</t>
+  </si>
+  <si>
+    <t>T44: {T=Integer, id=null},
+T45: {T=Integer, id=30}</t>
+  </si>
+  <si>
+    <t>T46: {latitude=-23.25},
+T47: {latitude=0},
+T48: {latitude=23.25}</t>
+  </si>
+  <si>
+    <t>T49: {longitude=-120.55},
+T50: {longitude=0},
+T51: {longitude=120.55}</t>
+  </si>
+  <si>
+    <t>T52: {time=-123},
+T53: {time=0},
+T54: {time=123}</t>
+  </si>
+  <si>
+    <t>T55: {R=String, value=empty string},
+T56: {R=String, value=2}</t>
+  </si>
+  <si>
+    <t>T57: {Info&lt;String, Integer&gt; (23.25, 120.55, 123, "2", Optional.of(null))},
+T58: {Info&lt;String, Integer&gt; (23.25, 120.55, 123, "2", Optional.of(30))}</t>
+  </si>
+  <si>
+    <t>T46: covers {latitude&lt;0},
+T47: covers {latitude=0},
+T48: covers {latitude&gt;0}</t>
+  </si>
+  <si>
+    <t>T49: covers {longitude&lt;0},
+T50: covers {longitude=0},
+T51: covers {longitude&gt;0}</t>
+  </si>
+  <si>
+    <t>T52: covers {time&lt;0},
+T53: covers {time=0},
+T54: covers {time&gt;0}</t>
+  </si>
+  <si>
+    <t>T55: covers {true},
+T56: covers {false}</t>
+  </si>
+  <si>
+    <t>T57: covers {true},
+T58: covers {false}</t>
+  </si>
+  <si>
+    <t>T42: {hash=null},
+T43: {hash=29jw}</t>
   </si>
 </sst>
 </file>
@@ -643,7 +727,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -933,8 +1017,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -974,8 +1101,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1042,6 +1175,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1060,38 +1211,31 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1375,19 +1519,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="16" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="71" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
@@ -1398,59 +1542,59 @@
     <col min="11" max="11" width="48.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.83203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="66" style="1" customWidth="1"/>
-    <col min="14" max="14" width="35.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="42.5" style="1" customWidth="1"/>
     <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="15" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="32" t="s">
+      <c r="C1" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="K1" s="32" t="s">
+      <c r="J1" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="192" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="22" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1491,7 +1635,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="112" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
@@ -1533,7 +1677,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="112" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="18" t="s">
         <v>31</v>
       </c>
@@ -1575,7 +1719,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="18" t="s">
         <v>32</v>
       </c>
@@ -1617,7 +1761,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="19" t="s">
         <v>46</v>
       </c>
@@ -1659,7 +1803,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="30" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -1681,7 +1825,7 @@
         <v>57</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>63</v>
@@ -1696,14 +1840,14 @@
         <v>14</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="N7" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="18" t="s">
         <v>66</v>
       </c>
@@ -1723,7 +1867,7 @@
         <v>67</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>68</v>
@@ -1738,14 +1882,14 @@
         <v>14</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="N8" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="18" t="s">
         <v>69</v>
       </c>
@@ -1765,7 +1909,7 @@
         <v>74</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>70</v>
@@ -1780,313 +1924,397 @@
         <v>14</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
+      <c r="B10" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="N10" s="11" t="s">
+      <c r="K10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N10" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="21" t="s">
+    <row r="11" spans="1:14" ht="176" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="8" t="s">
+      <c r="E13" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="K13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="N13" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
+      <c r="B15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
+      <c r="B16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="31"/>
+      <c r="B17" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="J15" s="8" t="s">
+      <c r="F18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>127</v>
+      <c r="K18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A13:A18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>